<commit_message>
Data from preliminary observation
</commit_message>
<xml_diff>
--- a/Data_Perf_Energy.xlsx
+++ b/Data_Perf_Energy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmukherjee/UIUC/Efficient_DVFS/osldvfs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC1449A-47E2-C046-8CA6-76E8648EFED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80A8E2D-2D1C-2E4E-907E-689899F96878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{C375F459-613A-E64E-A7C0-D28A192B58C4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Benchmark</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>time run 10 taskset -c 0 ./bfs</t>
+  </si>
+  <si>
+    <t>CPU Driven Gov</t>
+  </si>
+  <si>
+    <t>Mem Driven Gov</t>
+  </si>
+  <si>
+    <t>time run 10 taskset -c 0 ./sssp</t>
+  </si>
+  <si>
+    <t>GPU Driven Gov</t>
+  </si>
+  <si>
+    <t>time run 10  taskset -c 0 ./bfs</t>
   </si>
 </sst>
 </file>
@@ -176,11 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A1E52C-6EF9-A04F-A62B-2AB7DCD6CD38}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,40 +562,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>61.3</v>
-      </c>
-      <c r="E2">
-        <v>5.5</v>
-      </c>
-      <c r="F2">
-        <v>3.5</v>
-      </c>
-      <c r="G2">
-        <f>E2-F2</f>
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <f>C2*100/D2/G2</f>
-        <v>4.0783034257748776</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2">
-        <v>0.06</v>
-      </c>
-    </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
@@ -598,11 +582,11 @@
         <v>3.8</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G14" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G11" si="0">E3-F3</f>
         <v>2.7</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1">C3*100/D3/G3</f>
+        <f t="shared" ref="H3:H11" si="1">C3*100/D3/G3</f>
         <v>3.83477635967748</v>
       </c>
       <c r="I3" t="s">
@@ -651,33 +635,33 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>120.8</v>
+        <v>96.8</v>
       </c>
       <c r="E5">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="F5">
-        <v>3.3</v>
+        <v>3.7</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>2.8</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>3.7627934978928357</v>
+        <v>3.6894923258559627</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="J5">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -685,27 +669,27 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>96.8</v>
+        <v>193.62</v>
       </c>
       <c r="E6">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>3.6894923258559627</v>
+        <v>5.7386174522833961</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -714,38 +698,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>193.62</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>3.1</v>
-      </c>
-      <c r="G7">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>25.925999999999998</v>
+      </c>
+      <c r="E8">
+        <v>4.5</v>
+      </c>
+      <c r="F8">
+        <v>3.7</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="H7">
+        <v>0.79999999999999982</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>5.7386174522833961</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+        <v>24.107073979788638</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -753,33 +734,30 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>26.754999999999999</v>
+        <v>32.69</v>
       </c>
       <c r="E9">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F9">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0.89999999999999947</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>20.764550758944335</v>
+        <v>16.994663675605871</v>
       </c>
       <c r="I9" t="s">
         <v>21</v>
-      </c>
-      <c r="J9">
-        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -790,10 +768,10 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>25.925999999999998</v>
+        <v>52.05</v>
       </c>
       <c r="E10">
         <v>4.5</v>
@@ -807,10 +785,10 @@
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>24.107073979788638</v>
+        <v>24.015369836695491</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -821,126 +799,349 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>32.69</v>
+        <v>58.4</v>
       </c>
       <c r="E11">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="F11">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0.89999999999999947</v>
+        <v>0.90000000000000036</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>16.994663675605871</v>
+        <v>19.025875190258745</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>53.5</v>
-      </c>
-      <c r="E12">
-        <v>4.3</v>
-      </c>
-      <c r="F12">
-        <v>3.4</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>20.768431983385256</v>
-      </c>
-      <c r="I12" t="s">
         <v>23</v>
       </c>
-      <c r="J12">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>52.05</v>
-      </c>
-      <c r="E13">
-        <v>4.5</v>
-      </c>
-      <c r="F13">
-        <v>3.7</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0.79999999999999982</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>24.015369836695491</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>61.3</v>
+      </c>
+      <c r="E14">
+        <v>5.5</v>
+      </c>
+      <c r="F14">
+        <v>3.5</v>
+      </c>
+      <c r="G14">
+        <f>E14-F14</f>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f>C14*100/D14/G14</f>
+        <v>4.0783034257748776</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>120.8</v>
+      </c>
+      <c r="E15">
+        <v>5.5</v>
+      </c>
+      <c r="F15">
+        <v>3.3</v>
+      </c>
+      <c r="G15">
+        <f>E15-F15</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H15">
+        <f>C15*100/D15/G15</f>
+        <v>3.7627934978928357</v>
+      </c>
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>26.754999999999999</v>
+      </c>
+      <c r="E17">
+        <v>4.3</v>
+      </c>
+      <c r="F17">
+        <v>3.4</v>
+      </c>
+      <c r="G17">
+        <f>E17-F17</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H17">
+        <f>C17*100/D17/G17</f>
+        <v>20.764550758944335</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
         <v>10</v>
       </c>
-      <c r="D14">
-        <v>58.4</v>
-      </c>
-      <c r="E14">
-        <v>4.2</v>
-      </c>
-      <c r="F14">
-        <v>3.3</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0.90000000000000036</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>19.025875190258745</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="D18">
+        <v>53.5</v>
+      </c>
+      <c r="E18">
+        <v>4.3</v>
+      </c>
+      <c r="F18">
+        <v>3.4</v>
+      </c>
+      <c r="G18">
+        <f>E18-F18</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H18">
+        <f>C18*100/D18/G18</f>
+        <v>20.768431983385256</v>
+      </c>
+      <c r="I18" t="s">
         <v>23</v>
       </c>
+      <c r="J18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>58.8</v>
+      </c>
+      <c r="E20">
+        <v>6.3</v>
+      </c>
+      <c r="F20">
+        <v>3.9</v>
+      </c>
+      <c r="G20">
+        <f>E20-F20</f>
+        <v>2.4</v>
+      </c>
+      <c r="H20">
+        <f>C20*100/D20/G20</f>
+        <v>3.5430839002267578</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>129.9</v>
+      </c>
+      <c r="E21">
+        <v>6.6</v>
+      </c>
+      <c r="F21">
+        <v>3.8</v>
+      </c>
+      <c r="G21">
+        <f>E21-F21</f>
+        <v>2.8</v>
+      </c>
+      <c r="H21">
+        <f>C21*100/D21/G21</f>
+        <v>2.7493676454415485</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>47.18</v>
+      </c>
+      <c r="E23">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F23">
+        <v>3.7</v>
+      </c>
+      <c r="G23">
+        <f>E23-F23</f>
+        <v>0.89999999999999947</v>
+      </c>
+      <c r="H23">
+        <f>C23*100/D23/G23</f>
+        <v>11.775234327163119</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>94.55</v>
+      </c>
+      <c r="E24">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F24">
+        <v>3.7</v>
+      </c>
+      <c r="G24">
+        <f>E24-F24</f>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="H24">
+        <f>C24*100/D24/G24</f>
+        <v>15.10916370778877</v>
+      </c>
+      <c r="I24" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A13:J13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update to policy and script
</commit_message>
<xml_diff>
--- a/Data_Perf_Energy.xlsx
+++ b/Data_Perf_Energy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmukherjee/UIUC/Efficient_DVFS/osldvfs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24CC085-ACF9-7348-8052-A48C1766DDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10701C65-CA9F-5948-817E-18E75A2979C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{C375F459-613A-E64E-A7C0-D28A192B58C4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{C375F459-613A-E64E-A7C0-D28A192B58C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark--Perf--Energy" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Benchmark</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Chai : BFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,8 +856,8 @@
       <c r="C14">
         <v>5</v>
       </c>
-      <c r="D14">
-        <v>61.3</v>
+      <c r="D14" t="s">
+        <v>31</v>
       </c>
       <c r="E14">
         <v>5.5</v>
@@ -866,9 +869,9 @@
         <f>E14-F14</f>
         <v>2</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="e">
         <f>C14*100/D14/G14</f>
-        <v>4.0783034257748776</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>

</xml_diff>